<commit_message>
cambios en arca 13.08.2025
</commit_message>
<xml_diff>
--- a/Horarios2025_Version_07082025.xlsx
+++ b/Horarios2025_Version_07082025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00_ENGITHUB\Modulo02_JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36598F88-4DF3-412F-AA40-DC69795A008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D45C18-ED9A-4424-9712-446A7F770BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB16EAB-46E4-4296-9FB2-5DEE8DAED3CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="22">
   <si>
     <t>RECREO</t>
   </si>
@@ -88,13 +88,16 @@
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>SEGUNDO CUATRIMESTRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +128,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +174,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3DBFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -198,17 +221,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB2B772-8170-4FFE-ABA1-AFA216428B0A}">
-  <dimension ref="B1:R42"/>
+  <dimension ref="B2:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,107 +567,93 @@
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="H1" s="13" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="N1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="N2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
         <v>0.625</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>0.63194444444444442</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.63888888888888884</v>
-      </c>
-      <c r="D5" s="14"/>
       <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
@@ -651,10 +663,10 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C6" s="3">
         <v>0.63888888888888884</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.64583333333333337</v>
       </c>
       <c r="D6" s="14"/>
       <c r="J6" s="4" t="s">
@@ -666,10 +678,10 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>0.64583333333333304</v>
+        <v>0.63888888888888884</v>
       </c>
       <c r="C7" s="3">
-        <v>0.65277777777777801</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D7" s="14"/>
       <c r="J7" s="4" t="s">
@@ -681,10 +693,10 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="C8" s="3">
         <v>0.65277777777777801</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.65972222222222199</v>
       </c>
       <c r="D8" s="14"/>
       <c r="J8" s="4" t="s">
@@ -696,10 +708,10 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
+        <v>0.65277777777777801</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.65972222222222199</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.66666666666666696</v>
       </c>
       <c r="D9" s="14"/>
       <c r="J9" s="4" t="s">
@@ -711,87 +723,75 @@
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
+        <v>0.65972222222222199</v>
+      </c>
+      <c r="C10" s="3">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C10" s="3">
-        <v>0.67361111111111105</v>
-      </c>
       <c r="D10" s="14"/>
-      <c r="F10" s="15" t="s">
-        <v>4</v>
-      </c>
       <c r="J10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="C11" s="3">
         <v>0.67361111111111105</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="14"/>
+      <c r="F11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>0.67361111111111105</v>
+      </c>
+      <c r="C12" s="3">
         <v>0.68055555555555503</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="J11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R11" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="D12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="J12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <v>0.68055555555555503</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>0.6875</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="J12" s="6" t="s">
+      <c r="F13" s="13"/>
+      <c r="J13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P13" s="6" t="s">
         <v>0</v>
-      </c>
-      <c r="R12" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <v>0.6875</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.69444444444444398</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="J13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="R13" s="11" t="s">
         <v>18</v>
@@ -799,13 +799,15 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="C14" s="3">
         <v>0.69444444444444398</v>
       </c>
-      <c r="C14" s="3">
-        <v>0.70138888888888895</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="D14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="13"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
@@ -824,13 +826,13 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
+        <v>0.69444444444444398</v>
+      </c>
+      <c r="C15" s="3">
         <v>0.70138888888888895</v>
       </c>
-      <c r="C15" s="3">
-        <v>0.70833333333333304</v>
-      </c>
       <c r="D15" s="14"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="13"/>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
@@ -849,13 +851,13 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
+        <v>0.70138888888888895</v>
+      </c>
+      <c r="C16" s="3">
         <v>0.70833333333333304</v>
       </c>
-      <c r="C16" s="3">
-        <v>0.71527777777777701</v>
-      </c>
       <c r="D16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="13"/>
       <c r="J16" s="5" t="s">
         <v>17</v>
       </c>
@@ -874,13 +876,13 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="C17" s="3">
         <v>0.71527777777777701</v>
       </c>
-      <c r="C17" s="3">
-        <v>0.72222222222222199</v>
-      </c>
       <c r="D17" s="14"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="13"/>
       <c r="J17" s="5" t="s">
         <v>17</v>
       </c>
@@ -899,17 +901,15 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
+        <v>0.71527777777777701</v>
+      </c>
+      <c r="C18" s="3">
         <v>0.72222222222222199</v>
       </c>
-      <c r="C18" s="3">
-        <v>0.72916666666666596</v>
-      </c>
       <c r="D18" s="14"/>
-      <c r="F18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>0</v>
+      <c r="F18" s="13"/>
+      <c r="J18" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="L18" s="9" t="s">
         <v>16</v>
@@ -917,8 +917,8 @@
       <c r="N18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>0</v>
+      <c r="P18" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="R18" s="11" t="s">
         <v>18</v>
@@ -926,17 +926,17 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="C19" s="3">
         <v>0.72916666666666596</v>
       </c>
-      <c r="C19" s="3">
-        <v>0.73611111111111005</v>
-      </c>
       <c r="D19" s="14"/>
-      <c r="F19" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>17</v>
+      <c r="F19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L19" s="9" t="s">
         <v>16</v>
@@ -944,8 +944,8 @@
       <c r="N19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P19" s="5" t="s">
-        <v>17</v>
+      <c r="P19" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="R19" s="11" t="s">
         <v>18</v>
@@ -953,13 +953,15 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
-        <v>0.73611111111111105</v>
+        <v>0.72916666666666596</v>
       </c>
       <c r="C20" s="3">
-        <v>0.74305555555555503</v>
+        <v>0.73611111111111005</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="J20" s="5" t="s">
         <v>17</v>
       </c>
@@ -978,23 +980,21 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
+        <v>0.73611111111111105</v>
+      </c>
+      <c r="C21" s="3">
         <v>0.74305555555555503</v>
       </c>
-      <c r="C21" s="3">
-        <v>0.749999999999999</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="F21" s="13"/>
       <c r="J21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>0</v>
+      <c r="L21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>17</v>
@@ -1005,31 +1005,42 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>0.75</v>
+        <v>0.74305555555555503</v>
       </c>
       <c r="C22" s="3">
-        <v>0.75694444444444398</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="15"/>
+        <v>0.749999999999999</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="13"/>
       <c r="J22" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="L22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="P22" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="3">
         <v>0.75694444444444398</v>
       </c>
-      <c r="C23" s="3">
-        <v>0.76388888888888795</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="D23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="13"/>
       <c r="J23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1039,13 +1050,13 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
+        <v>0.75694444444444398</v>
+      </c>
+      <c r="C24" s="3">
         <v>0.76388888888888795</v>
       </c>
-      <c r="C24" s="3">
-        <v>0.77083333333333204</v>
-      </c>
       <c r="D24" s="14"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="13"/>
       <c r="J24" s="5" t="s">
         <v>17</v>
       </c>
@@ -1055,13 +1066,13 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>0.77083333333333304</v>
+        <v>0.76388888888888795</v>
       </c>
       <c r="C25" s="3">
-        <v>0.77777777777777701</v>
+        <v>0.77083333333333204</v>
       </c>
       <c r="D25" s="14"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="13"/>
       <c r="J25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1071,13 +1082,13 @@
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
+        <v>0.77083333333333304</v>
+      </c>
+      <c r="C26" s="3">
         <v>0.77777777777777701</v>
       </c>
-      <c r="C26" s="3">
-        <v>0.78472222222222099</v>
-      </c>
       <c r="D26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="13"/>
       <c r="J26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1087,46 +1098,43 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>0.78472222222222199</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="C27" s="3">
-        <v>0.79166666666666596</v>
+        <v>0.78472222222222099</v>
       </c>
       <c r="D27" s="14"/>
-      <c r="F27" s="2" t="s">
-        <v>0</v>
+      <c r="F27" s="13"/>
+      <c r="J27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
+        <v>0.78472222222222199</v>
+      </c>
+      <c r="C28" s="3">
         <v>0.79166666666666596</v>
       </c>
-      <c r="C28" s="3">
-        <v>0.79861111111111005</v>
-      </c>
       <c r="D28" s="14"/>
-      <c r="F28" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="11" t="s">
-        <v>18</v>
+      <c r="F28" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
+        <v>0.79166666666666596</v>
+      </c>
+      <c r="C29" s="3">
         <v>0.79861111111111005</v>
       </c>
-      <c r="C29" s="3">
-        <v>0.80555555555555403</v>
-      </c>
       <c r="D29" s="14"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="I29" s="11" t="s">
         <v>18</v>
       </c>
@@ -1139,13 +1147,13 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
-        <v>0.80555555555555558</v>
+        <v>0.79861111111111005</v>
       </c>
       <c r="C30" s="3">
-        <v>0.8125</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="F30" s="15"/>
+        <v>0.80555555555555403</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="F30" s="13"/>
       <c r="I30" s="11" t="s">
         <v>18</v>
       </c>
@@ -1158,13 +1166,13 @@
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="C31" s="3">
         <v>0.8125</v>
       </c>
-      <c r="C31" s="3">
-        <v>0.81944444444444442</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="F31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="F31" s="13"/>
       <c r="I31" s="11" t="s">
         <v>18</v>
       </c>
@@ -1177,13 +1185,13 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="C32" s="3">
         <v>0.81944444444444442</v>
       </c>
-      <c r="C32" s="3">
-        <v>0.82638888888888884</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="F32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="F32" s="13"/>
       <c r="I32" s="11" t="s">
         <v>18</v>
       </c>
@@ -1196,13 +1204,13 @@
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>0.82638888888888895</v>
+        <v>0.81944444444444442</v>
       </c>
       <c r="C33" s="3">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="F33" s="15"/>
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="F33" s="13"/>
       <c r="I33" s="11" t="s">
         <v>18</v>
       </c>
@@ -1211,23 +1219,17 @@
       </c>
       <c r="N33" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="R33" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
+        <v>0.82638888888888895</v>
+      </c>
+      <c r="C34" s="3">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C34" s="3">
-        <v>0.84027777777777801</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="F34" s="15"/>
-      <c r="H34" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="D34" s="15"/>
+      <c r="F34" s="13"/>
       <c r="I34" s="11" t="s">
         <v>18</v>
       </c>
@@ -1237,42 +1239,44 @@
       <c r="N34" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P34" s="11" t="s">
-        <v>18</v>
+      <c r="R34" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C35" s="3">
         <v>0.84027777777777801</v>
       </c>
-      <c r="C35" s="3">
+      <c r="D35" s="15"/>
+      <c r="F35" s="13"/>
+      <c r="H35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>0.84027777777777801</v>
+      </c>
+      <c r="C36" s="3">
         <v>0.84722222222222199</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="F35" s="15"/>
-      <c r="H35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P35" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="12">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="C36" s="12">
-        <v>0.85416666666666663</v>
-      </c>
+      <c r="D36" s="15"/>
+      <c r="F36" s="13"/>
       <c r="H36" s="11" t="s">
         <v>18</v>
       </c>
@@ -1291,94 +1295,118 @@
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="12">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C37" s="12">
         <v>0.85416666666666663</v>
       </c>
-      <c r="C37" s="3">
+      <c r="H37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="12">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C38" s="3">
         <v>0.86111111111111005</v>
       </c>
-      <c r="H37" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N37" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P37" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
+      <c r="H38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
         <v>0.86111111111111105</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C39" s="3">
         <v>0.86805555555555403</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P38" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
+      <c r="H39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="12">
         <v>0.86805555555555503</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C40" s="12">
         <v>0.874999999999998</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P39" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
+      <c r="H40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
     </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="N1:R2"/>
-    <mergeCell ref="F19:F26"/>
-    <mergeCell ref="F28:F35"/>
-    <mergeCell ref="D13:D20"/>
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="D30:D35"/>
-    <mergeCell ref="H1:L2"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="F10:F17"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="F20:F27"/>
+    <mergeCell ref="F29:F36"/>
+    <mergeCell ref="D14:D21"/>
+    <mergeCell ref="D23:D30"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="H2:L3"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="F11:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>